<commit_message>
updated cv: new position and updated talklist
</commit_message>
<xml_diff>
--- a/talklists/talklist.xlsx
+++ b/talklists/talklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sugiyamasunao/Documents/home/cv/talklists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C6622A-97CC-7A43-B2B1-E8D685F6E7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283E3F32-4CA1-154D-A89D-BDB65518C060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="135">
   <si>
     <t>title</t>
   </si>
@@ -603,12 +603,24 @@
   <si>
     <t>Cosmology analysis with Subaru HSC Y3 data and SDSS data: cosmological parameter inference in $\Lambda$CDM model</t>
   </si>
+  <si>
+    <t>HSC Year 3 Weak Lensing Cosmology Results</t>
+  </si>
+  <si>
+    <t>HSC webinar</t>
+  </si>
+  <si>
+    <t>https://hsc-release.mtk.nao.ac.jp/doc/index.php/wly3/</t>
+  </si>
+  <si>
+    <t>We presented our HSC-Y3 weak lensing cosmology results on webinar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -626,6 +638,12 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -755,10 +773,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -778,8 +797,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1941,7 +1963,7 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3029,24 +3051,42 @@
       <c r="R26" s="9"/>
     </row>
     <row r="27" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
+      <c r="A27" s="19" t="s">
+        <v>131</v>
+      </c>
       <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
+      <c r="C27" s="11">
+        <v>2023</v>
+      </c>
+      <c r="D27" s="11">
+        <v>4</v>
+      </c>
       <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="F27" s="19" t="s">
+        <v>132</v>
+      </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
+      <c r="J27" s="11">
+        <v>1</v>
+      </c>
+      <c r="K27" s="11">
+        <v>1</v>
+      </c>
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
+      <c r="O27" s="20" t="s">
+        <v>133</v>
+      </c>
       <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
+      <c r="Q27" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="R27" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
@@ -3211,6 +3251,7 @@
     <hyperlink ref="O24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="O25" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="O26" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="O27" r:id="rId22" xr:uid="{6A059B92-0398-DC4B-A4F2-1ECE66875F8F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
updated talk, referee, publications
</commit_message>
<xml_diff>
--- a/talklists/talklist.xlsx
+++ b/talklists/talklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sugiyamasunao/Documents/home/cv/talklists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A6D9CC-48AE-8740-B6E1-D771F649FDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0922C46-EBF8-4B45-9221-A29FF0D8FC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="183">
   <si>
     <t>title</t>
   </si>
@@ -734,6 +734,48 @@
   </si>
   <si>
     <t>DESI seminar telecon</t>
+  </si>
+  <si>
+    <t>Exploring Primordial Black Hole with Microlensing Data</t>
+  </si>
+  <si>
+    <t>Pacific conference</t>
+  </si>
+  <si>
+    <t>Alex Kusenko</t>
+  </si>
+  <si>
+    <t>https://pacific-conference.pa.ucla.edu/index.html</t>
+  </si>
+  <si>
+    <t>Focus week on primordial black holes 2024</t>
+  </si>
+  <si>
+    <t>https://indico.ipmu.jp/event/439/overview</t>
+  </si>
+  <si>
+    <t>Exploring Primordial Black Hole with Microlensing Data: Updates on Analysis Pipeline</t>
+  </si>
+  <si>
+    <t>UPenn CfPC workshop</t>
+  </si>
+  <si>
+    <t>UPenn</t>
+  </si>
+  <si>
+    <t>Allice, Valerio, Mengxiang</t>
+  </si>
+  <si>
+    <t>Cosmology with third-order shear statistics</t>
+  </si>
+  <si>
+    <t>Pasadena</t>
+  </si>
+  <si>
+    <t>UC Richard Gump Research Station</t>
+  </si>
+  <si>
+    <t>Roman F2F meeting</t>
   </si>
 </sst>
 </file>
@@ -929,7 +971,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -944,7 +986,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -972,6 +1013,11 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2103,11 +2149,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F28" sqref="F28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3177,7 +3223,7 @@
       <c r="R26" s="9"/>
     </row>
     <row r="27" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="27" t="s">
         <v>131</v>
       </c>
       <c r="B27" s="11"/>
@@ -3215,7 +3261,7 @@
       </c>
     </row>
     <row r="28" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="34" t="s">
         <v>135</v>
       </c>
       <c r="B28" s="8"/>
@@ -3258,40 +3304,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:18" s="34" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
+    <row r="29" spans="1:18" s="33" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31">
+      <c r="B29" s="29"/>
+      <c r="C29" s="30">
         <v>2023</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="30">
         <v>4</v>
       </c>
-      <c r="E29" s="32"/>
-      <c r="F29" s="29" t="s">
+      <c r="E29" s="31"/>
+      <c r="F29" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30">
-        <v>1</v>
-      </c>
-      <c r="K29" s="31">
-        <v>1</v>
-      </c>
-      <c r="L29" s="30"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="32"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="32"/>
-      <c r="R29" s="33"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29">
+        <v>1</v>
+      </c>
+      <c r="K29" s="30">
+        <v>1</v>
+      </c>
+      <c r="L29" s="29"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="32"/>
     </row>
     <row r="30" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="25" t="s">
         <v>163</v>
       </c>
       <c r="B30" s="8"/>
@@ -3301,10 +3347,10 @@
       <c r="D30" s="7">
         <v>4</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="25" t="s">
         <v>162</v>
       </c>
       <c r="G30" s="8"/>
@@ -3317,51 +3363,51 @@
       <c r="L30" s="8"/>
       <c r="M30" s="7"/>
       <c r="N30" s="6"/>
-      <c r="O30" s="27" t="s">
+      <c r="O30" s="26" t="s">
         <v>161</v>
       </c>
       <c r="P30" s="8"/>
-      <c r="Q30" s="26" t="s">
+      <c r="Q30" s="25" t="s">
         <v>164</v>
       </c>
       <c r="R30" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" s="34" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="29" t="s">
+    <row r="31" spans="1:18" s="33" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31">
+      <c r="B31" s="29"/>
+      <c r="C31" s="30">
         <v>2023</v>
       </c>
-      <c r="D31" s="31">
+      <c r="D31" s="30">
         <v>5</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29" t="s">
+      <c r="E31" s="28"/>
+      <c r="F31" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="G31" s="30"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30">
-        <v>1</v>
-      </c>
-      <c r="K31" s="31">
-        <v>1</v>
-      </c>
-      <c r="L31" s="30"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="32"/>
-      <c r="O31" s="36"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="29"/>
-      <c r="R31" s="33"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29">
+        <v>1</v>
+      </c>
+      <c r="K31" s="30">
+        <v>1</v>
+      </c>
+      <c r="L31" s="29"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="35"/>
+      <c r="P31" s="29"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="32"/>
     </row>
     <row r="32" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B32" s="8"/>
@@ -3371,8 +3417,8 @@
       <c r="D32" s="7">
         <v>5</v>
       </c>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26" t="s">
+      <c r="E32" s="25"/>
+      <c r="F32" s="25" t="s">
         <v>167</v>
       </c>
       <c r="G32" s="8"/>
@@ -3387,127 +3433,127 @@
       <c r="L32" s="8"/>
       <c r="M32" s="7"/>
       <c r="N32" s="6"/>
-      <c r="O32" s="27"/>
+      <c r="O32" s="26"/>
       <c r="P32" s="8"/>
-      <c r="Q32" s="26"/>
+      <c r="Q32" s="25"/>
       <c r="R32" s="13"/>
     </row>
-    <row r="33" spans="1:18" s="34" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="29" t="s">
+    <row r="33" spans="1:18" s="33" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31">
+      <c r="B33" s="29"/>
+      <c r="C33" s="30">
         <v>2023</v>
       </c>
-      <c r="D33" s="31">
+      <c r="D33" s="30">
         <v>6</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29" t="s">
+      <c r="E33" s="28"/>
+      <c r="F33" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="G33" s="30"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="30">
-        <v>1</v>
-      </c>
-      <c r="J33" s="30">
-        <v>1</v>
-      </c>
-      <c r="K33" s="31">
-        <v>1</v>
-      </c>
-      <c r="L33" s="30"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="29"/>
-      <c r="R33" s="33"/>
-    </row>
-    <row r="34" spans="1:18" s="41" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37" t="s">
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="29">
+        <v>1</v>
+      </c>
+      <c r="J33" s="29">
+        <v>1</v>
+      </c>
+      <c r="K33" s="30">
+        <v>1</v>
+      </c>
+      <c r="L33" s="29"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="29"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="32"/>
+    </row>
+    <row r="34" spans="1:18" s="40" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38">
+      <c r="B34" s="37"/>
+      <c r="C34" s="37">
         <v>2023</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D34" s="37">
         <v>8</v>
       </c>
-      <c r="E34" s="39" t="s">
+      <c r="E34" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="F34" s="39" t="s">
+      <c r="F34" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38">
-        <v>1</v>
-      </c>
-      <c r="I34" s="38"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="38">
-        <v>1</v>
-      </c>
-      <c r="L34" s="38"/>
-      <c r="M34" s="38">
-        <v>1</v>
-      </c>
-      <c r="N34" s="39" t="s">
+      <c r="G34" s="37"/>
+      <c r="H34" s="37">
+        <v>1</v>
+      </c>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37">
+        <v>1</v>
+      </c>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37">
+        <v>1</v>
+      </c>
+      <c r="N34" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="O34" s="40" t="s">
+      <c r="O34" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="P34" s="38"/>
-      <c r="Q34" s="38"/>
-      <c r="R34" s="38"/>
+      <c r="P34" s="37"/>
+      <c r="Q34" s="37"/>
+      <c r="R34" s="37"/>
     </row>
     <row r="35" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22">
+      <c r="B35" s="21"/>
+      <c r="C35" s="21">
         <v>2023</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="21">
         <v>10</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23" t="s">
+      <c r="E35" s="22"/>
+      <c r="F35" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22">
-        <v>1</v>
-      </c>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22">
-        <v>1</v>
-      </c>
-      <c r="K35" s="22">
-        <v>1</v>
-      </c>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="24" t="s">
+      <c r="G35" s="21"/>
+      <c r="H35" s="21">
+        <v>1</v>
+      </c>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21">
+        <v>1</v>
+      </c>
+      <c r="K35" s="21">
+        <v>1</v>
+      </c>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="23" t="s">
+      <c r="P35" s="21"/>
+      <c r="Q35" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="R35" s="25">
+      <c r="R35" s="24">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="20" t="s">
         <v>148</v>
       </c>
       <c r="B36" s="8"/>
@@ -3517,10 +3563,10 @@
       <c r="D36" s="8">
         <v>1</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="18" t="s">
         <v>146</v>
       </c>
       <c r="G36" s="8"/>
@@ -3537,15 +3583,17 @@
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
-      <c r="O36" s="20" t="s">
+      <c r="O36" s="19" t="s">
         <v>147</v>
       </c>
       <c r="P36" s="8"/>
       <c r="Q36" s="8"/>
-      <c r="R36" s="9"/>
+      <c r="R36" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="16" t="s">
         <v>149</v>
       </c>
       <c r="B37" s="11"/>
@@ -3555,10 +3603,10 @@
       <c r="D37" s="11">
         <v>2</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="F37" s="16" t="s">
         <v>151</v>
       </c>
       <c r="G37" s="11"/>
@@ -3572,16 +3620,18 @@
       </c>
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
-      <c r="N37" s="17" t="s">
+      <c r="N37" s="16" t="s">
         <v>152</v>
       </c>
       <c r="O37" s="11"/>
       <c r="P37" s="11"/>
       <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
+      <c r="R37" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="20" t="s">
         <v>148</v>
       </c>
       <c r="B38" s="8"/>
@@ -3591,10 +3641,10 @@
       <c r="D38" s="8">
         <v>5</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="18" t="s">
         <v>157</v>
       </c>
       <c r="G38" s="8"/>
@@ -3608,14 +3658,14 @@
       <c r="M38" s="8">
         <v>1</v>
       </c>
-      <c r="N38" s="17" t="s">
+      <c r="N38" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="O38" s="20" t="s">
+      <c r="O38" s="19" t="s">
         <v>159</v>
       </c>
       <c r="P38" s="8"/>
-      <c r="Q38" s="19" t="s">
+      <c r="Q38" s="18" t="s">
         <v>160</v>
       </c>
       <c r="R38" s="9">
@@ -3623,43 +3673,160 @@
       </c>
     </row>
     <row r="39" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
+      <c r="A39" s="16" t="s">
+        <v>169</v>
+      </c>
       <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+      <c r="C39" s="11">
+        <v>2024</v>
+      </c>
+      <c r="D39" s="11">
+        <v>8</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>170</v>
+      </c>
       <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
+      <c r="H39" s="11">
+        <v>1</v>
+      </c>
       <c r="I39" s="11"/>
       <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
+      <c r="K39" s="11">
+        <v>1</v>
+      </c>
       <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="O39" s="11"/>
+      <c r="M39" s="11">
+        <v>1</v>
+      </c>
+      <c r="N39" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="O39" s="42" t="s">
+        <v>172</v>
+      </c>
       <c r="P39" s="11"/>
       <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
+      <c r="R39" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="16"/>
+      <c r="A40" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21">
+        <v>2024</v>
+      </c>
+      <c r="D40" s="21">
+        <v>10</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21">
+        <v>1</v>
+      </c>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="41"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21">
+        <v>2024</v>
+      </c>
+      <c r="D41" s="21">
+        <v>11</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21">
+        <v>1</v>
+      </c>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21">
+        <v>1</v>
+      </c>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="O41" s="23"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14">
+        <v>2024</v>
+      </c>
+      <c r="D42" s="14">
+        <v>11</v>
+      </c>
+      <c r="E42" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14">
+        <v>1</v>
+      </c>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14">
+        <v>1</v>
+      </c>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14">
+        <v>1</v>
+      </c>
+      <c r="N42" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="O42" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="15">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3691,6 +3858,7 @@
     <hyperlink ref="O35" r:id="rId26" xr:uid="{86A01E5A-8DA1-6B49-9651-0D71C5894E40}"/>
     <hyperlink ref="O38" r:id="rId27" xr:uid="{F278CA5F-70C1-244D-8F8F-D544334D6DA0}"/>
     <hyperlink ref="O30" r:id="rId28" xr:uid="{355E5364-5F3C-FA46-9141-89019E4CF3B7}"/>
+    <hyperlink ref="O39" r:id="rId29" xr:uid="{C5D9AC31-DFAA-B44A-A853-C21314623C5C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>